<commit_message>
Update JSON data format to include game data and add lists for primary/secondary
</commit_message>
<xml_diff>
--- a/12/HVI/TEXAS_CAL.xlsx
+++ b/12/HVI/TEXAS_CAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raghu\quidditch\live-stats\12\HVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB627C6-4E8C-47CF-92F0-B78C323B0AAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C49E86-EA9D-4F2C-92D2-C90969BCB061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -739,7 +739,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -747,20 +755,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,21 +1012,21 @@
     <row r="1" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
       <c r="R1" s="2"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -1039,140 +1039,140 @@
     </row>
     <row r="2" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="26" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="26">
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="22">
         <f>COUNTIFS(A:A,"G*") + COUNTIFS(G:G,"G*")+COUNTIFS(M:M,"G*")+COUNTIFS(S:S,"G*")</f>
         <v>9</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="27" t="str">
+      <c r="M2" s="23"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="28" t="str">
         <f>IF(COUNTIF($A$7:$X$59,"RCA"),"*","")&amp;IF(COUNTIF($A$7:$X$59,"OCA"),"^","")&amp;IF(COUNTIF($R$7:$X$59,"2CA"),"!","")</f>
         <v>*</v>
       </c>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="18" t="str">
+      <c r="P2" s="23"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="29" t="str">
         <f>CONCATENATE(LEN(O2)*30+L2*10,O2)</f>
         <v>120*</v>
       </c>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="20"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="24"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="23"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="27"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="26">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="22">
         <f>COUNTIFS(D:D,"G*")+COUNTIFS(J:J,"G*")+COUNTIFS(P:P,"G*")+COUNTIFS(V:V,"G*")</f>
         <v>7</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="27" t="str">
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="28" t="str">
         <f>IF(COUNTIF($A$7:$R$59,"RCB"),"*","")&amp;IF(COUNTIF($A$7:$R$59,"OCB"),"^","")&amp;IF(COUNTIF($A$7:$R$59,"2CB"),"!","")</f>
         <v/>
       </c>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="18" t="str">
+      <c r="P4" s="23"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="29" t="str">
         <f>CONCATENATE(LEN(O4)*30+L4*10,O4)</f>
         <v>70</v>
       </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="20"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="24"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="23"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="27"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
@@ -29465,6 +29465,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="R2:W3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:H5"/>
+    <mergeCell ref="I4:K5"/>
+    <mergeCell ref="L4:N5"/>
+    <mergeCell ref="O4:Q5"/>
+    <mergeCell ref="R4:W5"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
@@ -29474,13 +29481,6 @@
     <mergeCell ref="I2:K3"/>
     <mergeCell ref="L2:N3"/>
     <mergeCell ref="O2:Q3"/>
-    <mergeCell ref="R2:W3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:H5"/>
-    <mergeCell ref="I4:K5"/>
-    <mergeCell ref="L4:N5"/>
-    <mergeCell ref="O4:Q5"/>
-    <mergeCell ref="R4:W5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -29495,8 +29495,8 @@
   </sheetPr>
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29605,6 +29605,9 @@
       <c r="A12" s="15">
         <v>10</v>
       </c>
+      <c r="C12" s="15" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
@@ -30087,9 +30090,7 @@
       <c r="B90" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C90" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="C90" s="15"/>
     </row>
     <row r="91" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">

</xml_diff>